<commit_message>
🌃Added cleaner night transition, and only rendering night effect on outside zones.
</commit_message>
<xml_diff>
--- a/data/world/WiredData.xlsx
+++ b/data/world/WiredData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magic\Desktop\Wired\data\world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644B46F3-5811-4A89-B516-F1E8BAC0DAD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC77AEEA-2183-4F3A-9064-AEDCF0AC915A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="NPCS" sheetId="2" r:id="rId2"/>
-    <sheet name="Trabajos" sheetId="3" r:id="rId3"/>
+    <sheet name="Tasks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
     <t>Cable UTP</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
     <t>Kike</t>
   </si>
   <si>
-    <t>Id NPC</t>
-  </si>
-  <si>
-    <t>Recompensa</t>
-  </si>
-  <si>
     <t>Conoce a tus amigos</t>
   </si>
   <si>
@@ -135,6 +126,198 @@
   </si>
   <si>
     <t>usb_double_cable</t>
+  </si>
+  <si>
+    <t>players_house</t>
+  </si>
+  <si>
+    <t>final_zone_id</t>
+  </si>
+  <si>
+    <t>initial_zone_id</t>
+  </si>
+  <si>
+    <t>school_museum</t>
+  </si>
+  <si>
+    <t>school_general</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>Fide</t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>altairs_house</t>
+  </si>
+  <si>
+    <t>chenchos_house</t>
+  </si>
+  <si>
+    <t>jordis_house</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Juliette</t>
+  </si>
+  <si>
+    <t>music_store</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Sabine</t>
+  </si>
+  <si>
+    <t>Ale</t>
+  </si>
+  <si>
+    <t>kat</t>
+  </si>
+  <si>
+    <t>hiram</t>
+  </si>
+  <si>
+    <t>altair</t>
+  </si>
+  <si>
+    <t>chencho</t>
+  </si>
+  <si>
+    <t>arian</t>
+  </si>
+  <si>
+    <t>jordi</t>
+  </si>
+  <si>
+    <t>kike</t>
+  </si>
+  <si>
+    <t>laura</t>
+  </si>
+  <si>
+    <t>javier</t>
+  </si>
+  <si>
+    <t>juliette</t>
+  </si>
+  <si>
+    <t>fide</t>
+  </si>
+  <si>
+    <t>julia</t>
+  </si>
+  <si>
+    <t>sabine</t>
+  </si>
+  <si>
+    <t>jatzin</t>
+  </si>
+  <si>
+    <t>ale</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>roy</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>letty</t>
+  </si>
+  <si>
+    <t>Letty</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>liz1</t>
+  </si>
+  <si>
+    <t>liz2</t>
+  </si>
+  <si>
+    <t>store</t>
+  </si>
+  <si>
+    <t>city_store</t>
+  </si>
+  <si>
+    <t>ricardo</t>
+  </si>
+  <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t>Reward</t>
+  </si>
+  <si>
+    <t>Advancement</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Habla con Roy</t>
+  </si>
+  <si>
+    <t>Crea 3 cables</t>
+  </si>
+  <si>
+    <t>Realiza tu primer trabajo de subneteo</t>
+  </si>
+  <si>
+    <t>Realiza tu primer trabajo de enrutamiento</t>
+  </si>
+  <si>
+    <t>Crea 3 cables, uno directo y 2 cruzados.</t>
+  </si>
+  <si>
+    <t>Explora el pueblo y la ciudad para conocer a tus amigos.</t>
+  </si>
+  <si>
+    <t>Dirigete al Hotel y realiza tu primer trabajo de Subneteo.</t>
+  </si>
+  <si>
+    <t>Dirigete al Supermercado y realiza tu primer trabajo de Enrutamiento</t>
+  </si>
+  <si>
+    <t>Regresa con Roy</t>
+  </si>
+  <si>
+    <t>Objetives</t>
+  </si>
+  <si>
+    <t>kat_known roy_known</t>
+  </si>
+  <si>
+    <t>player_has_crossover_2 player_has_direct_1</t>
+  </si>
+  <si>
+    <t>hotel_subnetting_done</t>
+  </si>
+  <si>
+    <t>roy_talk_1</t>
+  </si>
+  <si>
+    <t>roy_talk_2</t>
+  </si>
+  <si>
+    <t>supermarket_routing_done</t>
   </si>
 </sst>
 </file>
@@ -181,7 +364,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -204,11 +387,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -221,6 +415,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -539,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F7D82F-C7FA-48A0-A98C-E412AC99610D}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -558,27 +755,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="D2" s="4">
         <v>10</v>
@@ -587,13 +784,13 @@
     </row>
     <row r="3" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="4">
         <v>20</v>
@@ -602,13 +799,13 @@
     </row>
     <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
@@ -617,13 +814,13 @@
     </row>
     <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4">
@@ -632,13 +829,13 @@
     </row>
     <row r="6" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4">
@@ -647,13 +844,13 @@
     </row>
     <row r="7" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4">
@@ -662,13 +859,13 @@
     </row>
     <row r="8" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
@@ -677,13 +874,13 @@
     </row>
     <row r="9" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4">
@@ -692,13 +889,13 @@
     </row>
     <row r="10" spans="1:5" ht="36" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -808,162 +1005,289 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3E07F7-65FD-45A8-A214-9C5363908E3F}">
-  <dimension ref="A2:B22"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>0</v>
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4"/>
-    </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4"/>
-    </row>
-    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -972,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3A0007-EA5C-4A6A-96E9-DE9E7F963C70}">
-  <dimension ref="A2:E22"/>
+  <dimension ref="A2:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,83 +1307,135 @@
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>81</v>
+      </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1067,8 +1443,10 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1076,8 +1454,10 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1085,8 +1465,10 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1094,8 +1476,10 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1103,8 +1487,10 @@
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -1112,8 +1498,10 @@
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -1121,8 +1509,10 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -1130,8 +1520,10 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1139,8 +1531,10 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -1148,8 +1542,10 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -1157,8 +1553,10 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -1166,8 +1564,10 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -1175,8 +1575,10 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -1184,6 +1586,8 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
✅Added simple task system, added portrait animation to dialogue scene, split item loader
</commit_message>
<xml_diff>
--- a/data/world/WiredData.xlsx
+++ b/data/world/WiredData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magic\Desktop\Wired\data\world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC77AEEA-2183-4F3A-9064-AEDCF0AC915A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21491B79-8D4F-4D24-86BF-62469932AFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="NPCS" sheetId="2" r:id="rId2"/>
     <sheet name="Tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="Dialogues" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="118">
   <si>
     <t>Id</t>
   </si>
@@ -38,9 +39,6 @@
     <t>Cable de red, útil para la transmisión de voz y datos. Se utiliza para crear cables ethernet.</t>
   </si>
   <si>
-    <t>Plug RJ45</t>
-  </si>
-  <si>
     <t>Conector de 8 contactos, sirve para armar cables Ethernet y realizar instalaciones de red. Se usa al subnetear.</t>
   </si>
   <si>
@@ -68,9 +66,6 @@
     <t>Kike</t>
   </si>
   <si>
-    <t>Conoce a tus amigos</t>
-  </si>
-  <si>
     <t>UBS-Doble Cable</t>
   </si>
   <si>
@@ -263,33 +258,15 @@
     <t>Ricardo</t>
   </si>
   <si>
-    <t>Reward</t>
-  </si>
-  <si>
-    <t>Advancement</t>
-  </si>
-  <si>
-    <t>Progress</t>
-  </si>
-  <si>
     <t>Habla con Roy</t>
   </si>
   <si>
-    <t>Crea 3 cables</t>
-  </si>
-  <si>
     <t>Realiza tu primer trabajo de subneteo</t>
   </si>
   <si>
     <t>Realiza tu primer trabajo de enrutamiento</t>
   </si>
   <si>
-    <t>Crea 3 cables, uno directo y 2 cruzados.</t>
-  </si>
-  <si>
-    <t>Explora el pueblo y la ciudad para conocer a tus amigos.</t>
-  </si>
-  <si>
     <t>Dirigete al Hotel y realiza tu primer trabajo de Subneteo.</t>
   </si>
   <si>
@@ -299,16 +276,88 @@
     <t>Regresa con Roy</t>
   </si>
   <si>
-    <t>Objetives</t>
-  </si>
-  <si>
-    <t>kat_known roy_known</t>
-  </si>
-  <si>
-    <t>player_has_crossover_2 player_has_direct_1</t>
-  </si>
-  <si>
-    <t>hotel_subnetting_done</t>
+    <t>kat_known</t>
+  </si>
+  <si>
+    <t>npc_id</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Hola @, ve a conocer a Roy</t>
+  </si>
+  <si>
+    <t>Hola @, ve a conocer a Chencho</t>
+  </si>
+  <si>
+    <t>chencho_known</t>
+  </si>
+  <si>
+    <t>roy_known</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>Bienvenido a nuestro humilde pueblo</t>
+  </si>
+  <si>
+    <t>requirement</t>
+  </si>
+  <si>
+    <t>Hola @,  bienvenido a Routed. Inc., conoces los 3 objetos escondidos?, explora y los conoceras. Ahora ve a esa estación de trabajo y crea 2 cables cruzados y un cable directo</t>
+  </si>
+  <si>
+    <t>Conoce a Kat</t>
+  </si>
+  <si>
+    <t>Conoce a Chencho</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>subnetting</t>
+  </si>
+  <si>
+    <t>routing</t>
+  </si>
+  <si>
+    <t>Crea un cable directo</t>
+  </si>
+  <si>
+    <t>Crea dos cables cruzados</t>
+  </si>
+  <si>
+    <t>crossover_2</t>
+  </si>
+  <si>
+    <t>direct_1</t>
+  </si>
+  <si>
+    <t>consequence</t>
+  </si>
+  <si>
+    <t>supermarket</t>
+  </si>
+  <si>
+    <t>subnetting_hotel_done</t>
+  </si>
+  <si>
+    <t>routing_supermarket_done</t>
   </si>
   <si>
     <t>roy_talk_1</t>
@@ -317,7 +366,22 @@
     <t>roy_talk_2</t>
   </si>
   <si>
-    <t>supermarket_routing_done</t>
+    <t>direct_cable_tutorial</t>
+  </si>
+  <si>
+    <t>crossover_cable_tutorial</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>task_id</t>
+  </si>
+  <si>
+    <t>Conector RJ45</t>
   </si>
 </sst>
 </file>
@@ -402,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -417,8 +481,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -736,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F7D82F-C7FA-48A0-A98C-E412AC99610D}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -755,21 +822,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -784,13 +851,13 @@
     </row>
     <row r="3" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
       </c>
       <c r="D3" s="4">
         <v>20</v>
@@ -799,13 +866,13 @@
     </row>
     <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4">
@@ -814,13 +881,13 @@
     </row>
     <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4">
@@ -829,13 +896,13 @@
     </row>
     <row r="6" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4">
@@ -844,13 +911,13 @@
     </row>
     <row r="7" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4">
@@ -859,13 +926,13 @@
     </row>
     <row r="8" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4">
@@ -874,13 +941,13 @@
     </row>
     <row r="9" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4">
@@ -889,13 +956,13 @@
     </row>
     <row r="10" spans="1:5" ht="36" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1024,249 +1091,249 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>74</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>75</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1296,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3A0007-EA5C-4A6A-96E9-DE9E7F963C70}">
-  <dimension ref="A2:G22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,289 +1374,619 @@
     <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C18CE2-38E8-451F-BD8D-67DA76996040}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>0</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="D4" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>96</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>19</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
📷Added player portrait, simple main tasks
</commit_message>
<xml_diff>
--- a/data/world/WiredData.xlsx
+++ b/data/world/WiredData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magic\Desktop\Wired\data\world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21491B79-8D4F-4D24-86BF-62469932AFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443CD414-4308-4B76-A327-6691E5F5975B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="131">
   <si>
     <t>Id</t>
   </si>
@@ -261,15 +261,9 @@
     <t>Habla con Roy</t>
   </si>
   <si>
-    <t>Realiza tu primer trabajo de subneteo</t>
-  </si>
-  <si>
     <t>Realiza tu primer trabajo de enrutamiento</t>
   </si>
   <si>
-    <t>Dirigete al Hotel y realiza tu primer trabajo de Subneteo.</t>
-  </si>
-  <si>
     <t>Dirigete al Supermercado y realiza tu primer trabajo de Enrutamiento</t>
   </si>
   <si>
@@ -318,12 +312,6 @@
     <t>Hola @,  bienvenido a Routed. Inc., conoces los 3 objetos escondidos?, explora y los conoceras. Ahora ve a esa estación de trabajo y crea 2 cables cruzados y un cable directo</t>
   </si>
   <si>
-    <t>Conoce a Kat</t>
-  </si>
-  <si>
-    <t>Conoce a Chencho</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -354,9 +342,6 @@
     <t>supermarket</t>
   </si>
   <si>
-    <t>subnetting_hotel_done</t>
-  </si>
-  <si>
     <t>routing_supermarket_done</t>
   </si>
   <si>
@@ -382,6 +367,60 @@
   </si>
   <si>
     <t>Conector RJ45</t>
+  </si>
+  <si>
+    <t>meet_kat</t>
+  </si>
+  <si>
+    <t>meet_chencho</t>
+  </si>
+  <si>
+    <t>meet_roy</t>
+  </si>
+  <si>
+    <t>create_crossover_cable</t>
+  </si>
+  <si>
+    <t>create_straight_cable</t>
+  </si>
+  <si>
+    <t>reception</t>
+  </si>
+  <si>
+    <t>subnetting_reception</t>
+  </si>
+  <si>
+    <t>Bienvenido a Celestia</t>
+  </si>
+  <si>
+    <t>Has llegado a Celestia, tu nuevo hogar y lugar de trabajo. Te han hablado de Kat, una chica del lugar que te ayudara a comenzar tu nueva vida.</t>
+  </si>
+  <si>
+    <t>Kat ha mencionado a Chencho, un amigo de tu antigua vida que ahora vive tambien en Celestia. Toma el autobus y reunete con el en la ciudad.</t>
+  </si>
+  <si>
+    <t>Tu viejo amigo</t>
+  </si>
+  <si>
+    <t>Routed Inc</t>
+  </si>
+  <si>
+    <t>Te han hablado e Roy, uno de los empleados de Routed Inc, con quien ahora trabajaras, ve que tiene para decirte.</t>
+  </si>
+  <si>
+    <t>Has hablado con Roy y te ha dado tu primer trabajo en Routed Inc. Dirigete a la recepción de los edificios de la empresa, cerca de tu casa, y habla con Ale la encargada de la recepción.</t>
+  </si>
+  <si>
+    <t>El primer trabajo</t>
+  </si>
+  <si>
+    <t>Los misterios de Celestia</t>
+  </si>
+  <si>
+    <t>En multiples ocasiones has oido hablar de Celestia, y algunas cosas parecen envolver al pueblo en misterio. Habla con los habitantes del pueblo para conocer mas acerca del lugar y lo que puede haber detrás de el.</t>
+  </si>
+  <si>
+    <t>mysteries_of_celestia</t>
   </si>
 </sst>
 </file>
@@ -804,20 +843,20 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12.6" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="1"/>
     <col min="5" max="5" width="34" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -834,7 +873,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="33.6" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -849,12 +888,12 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -864,7 +903,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -879,7 +918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -894,7 +933,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="72" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -909,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -924,7 +963,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -939,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="54" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -954,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="36" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="33.6" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -967,7 +1006,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -976,7 +1015,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -985,7 +1024,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -994,7 +1033,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1003,7 +1042,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1012,14 +1051,14 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1028,7 +1067,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1037,7 +1076,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1046,7 +1085,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1055,7 +1094,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1078,15 +1117,15 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.109375" customWidth="1"/>
+    <col min="3" max="3" width="34.88671875" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1139,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -1112,7 +1151,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>50</v>
       </c>
@@ -1124,7 +1163,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1136,7 +1175,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -1148,7 +1187,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
@@ -1160,7 +1199,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
@@ -1172,7 +1211,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -1184,7 +1223,7 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
@@ -1196,7 +1235,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
@@ -1208,7 +1247,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -1220,7 +1259,7 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>56</v>
       </c>
@@ -1232,7 +1271,7 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>57</v>
       </c>
@@ -1244,7 +1283,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>58</v>
       </c>
@@ -1256,7 +1295,7 @@
       </c>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>60</v>
       </c>
@@ -1268,7 +1307,7 @@
       </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>61</v>
       </c>
@@ -1280,7 +1319,7 @@
       </c>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>62</v>
       </c>
@@ -1292,7 +1331,7 @@
       </c>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -1304,7 +1343,7 @@
       </c>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>65</v>
       </c>
@@ -1316,7 +1355,7 @@
       </c>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
@@ -1328,7 +1367,7 @@
       </c>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>74</v>
       </c>
@@ -1338,19 +1377,19 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1365,19 +1404,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3A0007-EA5C-4A6A-96E9-DE9E7F963C70}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
-    <col min="4" max="6" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5546875" customWidth="1"/>
+    <col min="4" max="6" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1388,194 +1427,196 @@
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>0</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="84" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>96</v>
+        <v>120</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>121</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="84" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>123</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>52</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>2</v>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>3</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>4</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>5</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="117.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>69</v>
+        <v>118</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>6</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="117.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>128</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="D8" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="D9" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1585,7 +1626,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1595,7 +1636,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1605,7 +1646,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1615,7 +1656,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1625,7 +1666,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1635,7 +1676,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1645,7 +1686,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1655,7 +1696,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1665,7 +1706,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1675,7 +1716,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1699,37 +1740,37 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1737,17 +1778,17 @@
         <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1755,19 +1796,19 @@
         <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="84" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1775,17 +1816,17 @@
         <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1793,17 +1834,17 @@
         <v>49</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1811,17 +1852,17 @@
         <v>52</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1829,17 +1870,17 @@
         <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1849,7 +1890,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1859,7 +1900,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1869,7 +1910,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1879,7 +1920,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1889,7 +1930,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1899,7 +1940,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1909,7 +1950,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1919,7 +1960,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1929,7 +1970,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1939,7 +1980,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1949,7 +1990,7 @@
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1959,7 +2000,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1969,7 +2010,7 @@
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1979,7 +2020,7 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>

</xml_diff>

<commit_message>
📓Added simple task and dialogue system
</commit_message>
<xml_diff>
--- a/data/world/WiredData.xlsx
+++ b/data/world/WiredData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magic\Desktop\Wired\data\world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443CD414-4308-4B76-A327-6691E5F5975B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A74AC-F7D4-48E1-A1AF-887C9B2056CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
     <sheet name="NPCS" sheetId="2" r:id="rId2"/>
     <sheet name="Tasks" sheetId="3" r:id="rId3"/>
     <sheet name="Dialogues" sheetId="4" r:id="rId4"/>
+    <sheet name="Jobs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="152">
   <si>
     <t>Id</t>
   </si>
@@ -285,142 +286,251 @@
     <t>type</t>
   </si>
   <si>
-    <t>Hola @, ve a conocer a Roy</t>
-  </si>
-  <si>
-    <t>Hola @, ve a conocer a Chencho</t>
-  </si>
-  <si>
     <t>chencho_known</t>
   </si>
   <si>
     <t>roy_known</t>
   </si>
   <si>
-    <t>unique</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>subnetting</t>
+  </si>
+  <si>
+    <t>routing</t>
+  </si>
+  <si>
+    <t>Crea un cable directo</t>
+  </si>
+  <si>
+    <t>Crea dos cables cruzados</t>
+  </si>
+  <si>
+    <t>consequence</t>
+  </si>
+  <si>
+    <t>supermarket</t>
+  </si>
+  <si>
+    <t>routing_supermarket_done</t>
+  </si>
+  <si>
+    <t>roy_talk_2</t>
+  </si>
+  <si>
+    <t>direct_cable_tutorial</t>
+  </si>
+  <si>
+    <t>crossover_cable_tutorial</t>
+  </si>
+  <si>
+    <t>objective</t>
+  </si>
+  <si>
+    <t>has</t>
+  </si>
+  <si>
+    <t>Conector RJ45</t>
+  </si>
+  <si>
+    <t>meet_kat</t>
+  </si>
+  <si>
+    <t>meet_chencho</t>
+  </si>
+  <si>
+    <t>meet_roy</t>
+  </si>
+  <si>
+    <t>create_crossover_cable</t>
+  </si>
+  <si>
+    <t>create_straight_cable</t>
+  </si>
+  <si>
+    <t>reception</t>
+  </si>
+  <si>
+    <t>subnetting_reception</t>
+  </si>
+  <si>
+    <t>Bienvenido a Celestia</t>
+  </si>
+  <si>
+    <t>Has llegado a Celestia, tu nuevo hogar y lugar de trabajo. Te han hablado de Kat, una chica del lugar que te ayudara a comenzar tu nueva vida.</t>
+  </si>
+  <si>
+    <t>Kat ha mencionado a Chencho, un amigo de tu antigua vida que ahora vive tambien en Celestia. Toma el autobus y reunete con el en la ciudad.</t>
+  </si>
+  <si>
+    <t>Tu viejo amigo</t>
+  </si>
+  <si>
+    <t>Routed Inc</t>
+  </si>
+  <si>
+    <t>Te han hablado e Roy, uno de los empleados de Routed Inc, con quien ahora trabajaras, ve que tiene para decirte.</t>
+  </si>
+  <si>
+    <t>Has hablado con Roy y te ha dado tu primer trabajo en Routed Inc. Dirigete a la recepción de los edificios de la empresa, cerca de tu casa, y habla con Ale la encargada de la recepción.</t>
+  </si>
+  <si>
+    <t>El primer trabajo</t>
+  </si>
+  <si>
+    <t>Los misterios de Celestia</t>
+  </si>
+  <si>
+    <t>En multiples ocasiones has oido hablar de Celestia, y algunas cosas parecen envolver al pueblo en misterio. Habla con los habitantes del pueblo para conocer mas acerca del lugar y lo que puede haber detrás de el.</t>
+  </si>
+  <si>
+    <t>mysteries_of_celestia</t>
+  </si>
+  <si>
+    <t>npcs</t>
+  </si>
+  <si>
+    <t>Hola @, bienvenido a Celestia
+eres el nuevo trabajador de
+Routed Inc?
+Yo soy Kat, he vivido aqui toda mi vida
+Es bueno ver una cara nueva.
+Por que no tomas el autobus a la ciudad?
+Chencho te esta esperando ahi.
+Cuidate.</t>
+  </si>
+  <si>
+    <t>Holaaaaaa
+Que bueno verte de nuevo
+Pense que nunca volverias
+Escuche que te contrataron en Routed Inc
+Dicen que es un buen lugar para trabajar
+Pero a mi me da mala espina
+De cualquier forma, Roy tambien esta ahi
+Por que no pasas a saludarlo?
+Asi conoces tu nuevo lugar de trabajo</t>
+  </si>
+  <si>
+    <t>Hola @, vienes de Routed Inc?
+Soy Ale, trabajo aqui, me dijeron que vendrias
+Trabajaras en el subneteo de
+estos departamentos no es asi?
+Aqui hay 2 cuartos por lo que necesitaras:
+1 cable cruzado y 2 directos,
+asegurate de traerlos antes de hacer el subneteo.
+La mesa de trabajo esta a lado de esas cajas.</t>
+  </si>
+  <si>
+    <t>Perfecto, tu primer trabajo sera
+en un lugar cerca de tu casa.
+En los departamentos de la empresa
+habla con Ale, ella te dira mas.</t>
+  </si>
+  <si>
+    <t>mission</t>
+  </si>
+  <si>
+    <t>chencho
+kat</t>
+  </si>
+  <si>
+    <t>chencho
+kat
+roy</t>
+  </si>
+  <si>
+    <t>mission_requirement</t>
+  </si>
+  <si>
+    <t>meet_kat 1</t>
+  </si>
+  <si>
+    <t>meet_roy 1</t>
+  </si>
+  <si>
+    <t>subnetting_1</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>exercise</t>
+  </si>
+  <si>
+    <t>subnetting_1 0</t>
+  </si>
+  <si>
+    <t>subnetting_1 1</t>
+  </si>
+  <si>
+    <t>Ya quedó, muchísimas gracias
+Ya has recibido la paga por tu trabajo.</t>
+  </si>
+  <si>
+    <t>Escuche que te fue de maravilla
+Tendras un futuro exitoso!
+Tu siguiente tarea en realidad son
+varias tareas.
+Explora la ciudad y el pueblo
+completando estos trabajos
+para la empresa.
+Muchas felicidades!</t>
+  </si>
+  <si>
+    <t>meet_chencho 1</t>
+  </si>
+  <si>
+    <t>Ya has hablado con Chencho?</t>
+  </si>
+  <si>
+    <t>meet_chencho 0</t>
+  </si>
+  <si>
+    <t>mission_complete</t>
+  </si>
+  <si>
+    <t>Espero que te haya ido bien en tu primer dia</t>
   </si>
   <si>
     <t>generic</t>
   </si>
   <si>
-    <t>Bienvenido a nuestro humilde pueblo</t>
-  </si>
-  <si>
-    <t>requirement</t>
-  </si>
-  <si>
-    <t>Hola @,  bienvenido a Routed. Inc., conoces los 3 objetos escondidos?, explora y los conoceras. Ahora ve a esa estación de trabajo y crea 2 cables cruzados y un cable directo</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>talk</t>
-  </si>
-  <si>
-    <t>subnetting</t>
-  </si>
-  <si>
-    <t>routing</t>
-  </si>
-  <si>
-    <t>Crea un cable directo</t>
-  </si>
-  <si>
-    <t>Crea dos cables cruzados</t>
-  </si>
-  <si>
-    <t>crossover_2</t>
-  </si>
-  <si>
-    <t>direct_1</t>
-  </si>
-  <si>
-    <t>consequence</t>
-  </si>
-  <si>
-    <t>supermarket</t>
-  </si>
-  <si>
-    <t>routing_supermarket_done</t>
-  </si>
-  <si>
-    <t>roy_talk_1</t>
-  </si>
-  <si>
-    <t>roy_talk_2</t>
-  </si>
-  <si>
-    <t>direct_cable_tutorial</t>
-  </si>
-  <si>
-    <t>crossover_cable_tutorial</t>
-  </si>
-  <si>
-    <t>objective</t>
-  </si>
-  <si>
-    <t>has</t>
-  </si>
-  <si>
-    <t>task_id</t>
-  </si>
-  <si>
-    <t>Conector RJ45</t>
-  </si>
-  <si>
-    <t>meet_kat</t>
-  </si>
-  <si>
-    <t>meet_chencho</t>
-  </si>
-  <si>
-    <t>meet_roy</t>
-  </si>
-  <si>
-    <t>create_crossover_cable</t>
-  </si>
-  <si>
-    <t>create_straight_cable</t>
-  </si>
-  <si>
-    <t>reception</t>
-  </si>
-  <si>
-    <t>subnetting_reception</t>
-  </si>
-  <si>
-    <t>Bienvenido a Celestia</t>
-  </si>
-  <si>
-    <t>Has llegado a Celestia, tu nuevo hogar y lugar de trabajo. Te han hablado de Kat, una chica del lugar que te ayudara a comenzar tu nueva vida.</t>
-  </si>
-  <si>
-    <t>Kat ha mencionado a Chencho, un amigo de tu antigua vida que ahora vive tambien en Celestia. Toma el autobus y reunete con el en la ciudad.</t>
-  </si>
-  <si>
-    <t>Tu viejo amigo</t>
-  </si>
-  <si>
-    <t>Routed Inc</t>
-  </si>
-  <si>
-    <t>Te han hablado e Roy, uno de los empleados de Routed Inc, con quien ahora trabajaras, ve que tiene para decirte.</t>
-  </si>
-  <si>
-    <t>Has hablado con Roy y te ha dado tu primer trabajo en Routed Inc. Dirigete a la recepción de los edificios de la empresa, cerca de tu casa, y habla con Ale la encargada de la recepción.</t>
-  </si>
-  <si>
-    <t>El primer trabajo</t>
-  </si>
-  <si>
-    <t>Los misterios de Celestia</t>
-  </si>
-  <si>
-    <t>En multiples ocasiones has oido hablar de Celestia, y algunas cosas parecen envolver al pueblo en misterio. Habla con los habitantes del pueblo para conocer mas acerca del lugar y lo que puede haber detrás de el.</t>
-  </si>
-  <si>
-    <t>mysteries_of_celestia</t>
+    <t>new_mission</t>
+  </si>
+  <si>
+    <t>Hola</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @, bienvenido a Routed Inc!
+Yo soy Roy
+Antes de darte un trabajo
+Prueba las estaciones de trabajo
+Para practicar tus habilidades en Redes!
+En especial la de crear cables y
+subnetear, te seran de ayuda
+en tu proximo trabajo.
+Por que no creas:
+1 cable directo?</t>
+  </si>
+  <si>
+    <t>Perfecto, ahora crea:
+2 cables cruzados</t>
+  </si>
+  <si>
+    <t>create_crossover_cable 1</t>
+  </si>
+  <si>
+    <t>create_straight_cable 1</t>
+  </si>
+  <si>
+    <t>cable_straight 1</t>
+  </si>
+  <si>
+    <t>cable_crossover 2</t>
   </si>
 </sst>
 </file>
@@ -842,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F7D82F-C7FA-48A0-A98C-E412AC99610D}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -893,7 +1003,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -1402,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3A0007-EA5C-4A6A-96E9-DE9E7F963C70}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1413,10 +1523,13 @@
     <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5546875" customWidth="1"/>
-    <col min="4" max="6" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="6" max="7" width="30.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1427,156 +1540,191 @@
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="84" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="C2" s="4" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="84" x14ac:dyDescent="0.3">
+      <c r="H2" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="67.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="67.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="4" t="str">
+        <f>A5</f>
+        <v>create_straight_cable</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" s="4" t="str">
+        <f>A6</f>
+        <v>create_crossover_cable</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H6" s="4" t="str">
+        <f>A7</f>
+        <v>subnetting_reception</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="117.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="D7" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="117.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="117.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="117.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1587,16 +1735,18 @@
         <v>78</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>103</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1607,16 +1757,18 @@
         <v>76</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G10" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1625,8 +1777,10 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1635,8 +1789,10 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1645,8 +1801,10 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1655,8 +1813,10 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1665,8 +1825,10 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1675,8 +1837,10 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1685,8 +1849,10 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1695,8 +1861,10 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1705,8 +1873,10 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1715,8 +1885,10 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1725,6 +1897,11 @@
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H22" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1734,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C18CE2-38E8-451F-BD8D-67DA76996040}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,9 +1922,9 @@
     <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1764,13 +1941,13 @@
         <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1778,17 +1955,19 @@
         <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1796,19 +1975,19 @@
         <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="84" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="168" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1816,143 +1995,201 @@
         <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="F4" s="4" t="str">
+        <f>Tasks!A5</f>
+        <v>create_straight_cable</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="4" t="str">
+        <f>Tasks!A6</f>
+        <v>create_crossover_cable</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
+      <c r="B7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="134.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>7</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>135</v>
+      </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1962,7 +2199,7 @@
     </row>
     <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1972,7 +2209,7 @@
     </row>
     <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1982,7 +2219,7 @@
     </row>
     <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1992,7 +2229,7 @@
     </row>
     <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2002,7 +2239,7 @@
     </row>
     <row r="20" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2012,7 +2249,7 @@
     </row>
     <row r="21" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2020,14 +2257,61 @@
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+    <row r="22" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>19</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11805F5C-BCF8-41BF-8673-F0322C44C4C2}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
📠Fixed task system, NPCs without dialogs can return a default dialog
</commit_message>
<xml_diff>
--- a/data/world/WiredData.xlsx
+++ b/data/world/WiredData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magic\Desktop\Wired\data\world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A74AC-F7D4-48E1-A1AF-887C9B2056CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DBAD83-B29B-4559-BE9F-B84C5F0B2776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="160">
   <si>
     <t>Id</t>
   </si>
@@ -325,9 +325,6 @@
     <t>direct_cable_tutorial</t>
   </si>
   <si>
-    <t>crossover_cable_tutorial</t>
-  </si>
-  <si>
     <t>objective</t>
   </si>
   <si>
@@ -377,9 +374,6 @@
   </si>
   <si>
     <t>Has hablado con Roy y te ha dado tu primer trabajo en Routed Inc. Dirigete a la recepción de los edificios de la empresa, cerca de tu casa, y habla con Ale la encargada de la recepción.</t>
-  </si>
-  <si>
-    <t>El primer trabajo</t>
   </si>
   <si>
     <t>Los misterios de Celestia</t>
@@ -431,9 +425,6 @@
 habla con Ale, ella te dira mas.</t>
   </si>
   <si>
-    <t>mission</t>
-  </si>
-  <si>
     <t>chencho
 kat</t>
   </si>
@@ -459,12 +450,6 @@
   </si>
   <si>
     <t>exercise</t>
-  </si>
-  <si>
-    <t>subnetting_1 0</t>
-  </si>
-  <si>
-    <t>subnetting_1 1</t>
   </si>
   <si>
     <t>Ya quedó, muchísimas gracias
@@ -497,12 +482,6 @@
   </si>
   <si>
     <t>generic</t>
-  </si>
-  <si>
-    <t>new_mission</t>
-  </si>
-  <si>
-    <t>Hola</t>
   </si>
   <si>
     <t xml:space="preserve"> @, bienvenido a Routed Inc!
@@ -521,16 +500,61 @@
 2 cables cruzados</t>
   </si>
   <si>
-    <t>create_crossover_cable 1</t>
-  </si>
-  <si>
-    <t>create_straight_cable 1</t>
-  </si>
-  <si>
     <t>cable_straight 1</t>
   </si>
   <si>
     <t>cable_crossover 2</t>
+  </si>
+  <si>
+    <t>next_task</t>
+  </si>
+  <si>
+    <t>Cuentale a Roy que has creado un cable directo!</t>
+  </si>
+  <si>
+    <t>roy_crossover_cable</t>
+  </si>
+  <si>
+    <t>Cuentale a Roy que has creado dos cables cruzados!</t>
+  </si>
+  <si>
+    <t>meet_ale</t>
+  </si>
+  <si>
+    <t>Habla con Ale</t>
+  </si>
+  <si>
+    <t>Subnetea la red de la Recepcíon</t>
+  </si>
+  <si>
+    <t>roy_subnetting_reception</t>
+  </si>
+  <si>
+    <t>Vuelve con Roy</t>
+  </si>
+  <si>
+    <t>Ale te ha contado de que va este nuevo trabajo, tienes que realizar el subneteo de la Recepción, asegurate de tener los cables necesarios para comenzar.</t>
+  </si>
+  <si>
+    <t>Has terminado tu primer trabajo de subneto, vuelve a contarselo a Roy.</t>
+  </si>
+  <si>
+    <t>roy_straight_cable 1</t>
+  </si>
+  <si>
+    <t>roy_crossover_cable 1</t>
+  </si>
+  <si>
+    <t>meet_ale 1</t>
+  </si>
+  <si>
+    <t>subnetting_reception 1</t>
+  </si>
+  <si>
+    <t>roy_subnetting_reception 1</t>
+  </si>
+  <si>
+    <t>roy_straight_cable</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1027,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -1512,15 +1536,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3A0007-EA5C-4A6A-96E9-DE9E7F963C70}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.5546875" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
@@ -1543,27 +1567,27 @@
         <v>87</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>109</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>110</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>88</v>
@@ -1578,24 +1602,24 @@
         <v>80</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="84" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>52</v>
@@ -1604,24 +1628,24 @@
         <v>85</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>65</v>
@@ -1636,7 +1660,7 @@
     </row>
     <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>91</v>
@@ -1645,180 +1669,232 @@
         <v>91</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>97</v>
       </c>
       <c r="H5" s="4" t="str">
         <f>A6</f>
-        <v>create_crossover_cable</v>
+        <v>roy_straight_cable</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>105</v>
+        <v>159</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>98</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="4" t="str">
         <f>A7</f>
-        <v>subnetting_reception</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="117.6" x14ac:dyDescent="0.3">
+        <v>create_crossover_cable</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="4"/>
+        <v>99</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="117.6" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="str">
+        <f>A8</f>
+        <v>roy_crossover_cable</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>7</v>
+      <c r="H8" s="4" t="str">
+        <f>A9</f>
+        <v>meet_ale</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="117.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E9" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="F9" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>8</v>
+        <v>63</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="str">
+        <f>A10</f>
+        <v>subnetting_reception</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>79</v>
+        <v>149</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>76</v>
+        <v>152</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4" t="str">
+        <f>A11</f>
+        <v>roy_subnetting_reception</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>9</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+    <row r="12" spans="1:8" ht="117.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>11</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>12</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="F14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1830,7 +1906,7 @@
     </row>
     <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1842,7 +1918,7 @@
     </row>
     <row r="17" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1854,7 +1930,7 @@
     </row>
     <row r="18" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1866,7 +1942,7 @@
     </row>
     <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1878,7 +1954,7 @@
     </row>
     <row r="20" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1890,7 +1966,7 @@
     </row>
     <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1901,7 +1977,55 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
       <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="H26" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1911,10 +2035,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C18CE2-38E8-451F-BD8D-67DA76996040}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1924,10 +2048,9 @@
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -1941,13 +2064,10 @@
         <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1955,19 +2075,16 @@
         <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1975,19 +2092,16 @@
         <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="168" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="168" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1995,20 +2109,16 @@
         <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="4" t="str">
-        <f>Tasks!A5</f>
-        <v>create_straight_cable</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2016,178 +2126,145 @@
         <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="F5" s="4" t="str">
-        <f>Tasks!A6</f>
-        <v>create_crossover_cable</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="67.2" x14ac:dyDescent="0.3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="67.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="E8" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" ht="134.4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="134.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>143</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>143</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>143</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -2195,9 +2272,8 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -2205,9 +2281,8 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -2215,9 +2290,8 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -2225,9 +2299,8 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -2235,9 +2308,8 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2245,9 +2317,8 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -2255,9 +2326,8 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -2265,9 +2335,8 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -2294,18 +2363,18 @@
         <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>

<commit_message>
🗣️ Functional dialog system with options to give items or add tasks
</commit_message>
<xml_diff>
--- a/data/world/WiredData.xlsx
+++ b/data/world/WiredData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magic\Desktop\Wired\data\world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DBAD83-B29B-4559-BE9F-B84C5F0B2776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F9E3AC-86AE-4A9D-9DFF-2DDA6A385AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="172">
   <si>
     <t>Id</t>
   </si>
@@ -314,12 +314,6 @@
   </si>
   <si>
     <t>supermarket</t>
-  </si>
-  <si>
-    <t>routing_supermarket_done</t>
-  </si>
-  <si>
-    <t>roy_talk_2</t>
   </si>
   <si>
     <t>direct_cable_tutorial</t>
@@ -398,6 +392,141 @@
 Cuidate.</t>
   </si>
   <si>
+    <t>Hola @, vienes de Routed Inc?
+Soy Ale, trabajo aqui, me dijeron que vendrias
+Trabajaras en el subneteo de
+estos departamentos no es asi?
+Aqui hay 2 cuartos por lo que necesitaras:
+1 cable cruzado y 2 directos,
+asegurate de traerlos antes de hacer el subneteo.
+La mesa de trabajo esta a lado de esas cajas.</t>
+  </si>
+  <si>
+    <t>Perfecto, tu primer trabajo sera
+en un lugar cerca de tu casa.
+En los departamentos de la empresa
+habla con Ale, ella te dira mas.</t>
+  </si>
+  <si>
+    <t>chencho
+kat</t>
+  </si>
+  <si>
+    <t>chencho
+kat
+roy</t>
+  </si>
+  <si>
+    <t>mission_requirement</t>
+  </si>
+  <si>
+    <t>meet_kat 1</t>
+  </si>
+  <si>
+    <t>meet_roy 1</t>
+  </si>
+  <si>
+    <t>subnetting_1</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>exercise</t>
+  </si>
+  <si>
+    <t>Escuche que te fue de maravilla
+Tendras un futuro exitoso!
+Tu siguiente tarea en realidad son
+varias tareas.
+Explora la ciudad y el pueblo
+completando estos trabajos
+para la empresa.
+Muchas felicidades!</t>
+  </si>
+  <si>
+    <t>meet_chencho 1</t>
+  </si>
+  <si>
+    <t>Ya has hablado con Chencho?</t>
+  </si>
+  <si>
+    <t>meet_chencho 0</t>
+  </si>
+  <si>
+    <t>mission_complete</t>
+  </si>
+  <si>
+    <t>Espero que te haya ido bien en tu primer dia</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>Perfecto, ahora crea:
+2 cables cruzados</t>
+  </si>
+  <si>
+    <t>cable_straight 1</t>
+  </si>
+  <si>
+    <t>cable_crossover 2</t>
+  </si>
+  <si>
+    <t>next_task</t>
+  </si>
+  <si>
+    <t>Cuentale a Roy que has creado un cable directo!</t>
+  </si>
+  <si>
+    <t>roy_crossover_cable</t>
+  </si>
+  <si>
+    <t>Cuentale a Roy que has creado dos cables cruzados!</t>
+  </si>
+  <si>
+    <t>meet_ale</t>
+  </si>
+  <si>
+    <t>Habla con Ale</t>
+  </si>
+  <si>
+    <t>Subnetea la red de la Recepcíon</t>
+  </si>
+  <si>
+    <t>roy_subnetting_reception</t>
+  </si>
+  <si>
+    <t>Vuelve con Roy</t>
+  </si>
+  <si>
+    <t>Ale te ha contado de que va este nuevo trabajo, tienes que realizar el subneteo de la Recepción, asegurate de tener los cables necesarios para comenzar.</t>
+  </si>
+  <si>
+    <t>Has terminado tu primer trabajo de subneto, vuelve a contarselo a Roy.</t>
+  </si>
+  <si>
+    <t>roy_straight_cable 1</t>
+  </si>
+  <si>
+    <t>roy_crossover_cable 1</t>
+  </si>
+  <si>
+    <t>meet_ale 1</t>
+  </si>
+  <si>
+    <t>subnetting_reception 1</t>
+  </si>
+  <si>
+    <t>roy_subnetting_reception 1</t>
+  </si>
+  <si>
+    <t>roy_straight_cable</t>
+  </si>
+  <si>
+    <t>add_mission</t>
+  </si>
+  <si>
     <t>Holaaaaaa
 Que bueno verte de nuevo
 Pense que nunca volverias
@@ -406,85 +535,39 @@
 Pero a mi me da mala espina
 De cualquier forma, Roy tambien esta ahi
 Por que no pasas a saludarlo?
-Asi conoces tu nuevo lugar de trabajo</t>
-  </si>
-  <si>
-    <t>Hola @, vienes de Routed Inc?
-Soy Ale, trabajo aqui, me dijeron que vendrias
-Trabajaras en el subneteo de
-estos departamentos no es asi?
-Aqui hay 2 cuartos por lo que necesitaras:
-1 cable cruzado y 2 directos,
-asegurate de traerlos antes de hacer el subneteo.
-La mesa de trabajo esta a lado de esas cajas.</t>
-  </si>
-  <si>
-    <t>Perfecto, tu primer trabajo sera
-en un lugar cerca de tu casa.
-En los departamentos de la empresa
-habla con Ale, ella te dira mas.</t>
-  </si>
-  <si>
-    <t>chencho
-kat</t>
-  </si>
-  <si>
-    <t>chencho
-kat
-roy</t>
-  </si>
-  <si>
-    <t>mission_requirement</t>
-  </si>
-  <si>
-    <t>meet_kat 1</t>
-  </si>
-  <si>
-    <t>meet_roy 1</t>
-  </si>
-  <si>
-    <t>subnetting_1</t>
-  </si>
-  <si>
-    <t>zone</t>
-  </si>
-  <si>
-    <t>exercise</t>
-  </si>
-  <si>
-    <t>Ya quedó, muchísimas gracias
-Ya has recibido la paga por tu trabajo.</t>
-  </si>
-  <si>
-    <t>Escuche que te fue de maravilla
-Tendras un futuro exitoso!
-Tu siguiente tarea en realidad son
-varias tareas.
-Explora la ciudad y el pueblo
-completando estos trabajos
-para la empresa.
-Muchas felicidades!</t>
-  </si>
-  <si>
-    <t>meet_chencho 1</t>
-  </si>
-  <si>
-    <t>Ya has hablado con Chencho?</t>
-  </si>
-  <si>
-    <t>meet_chencho 0</t>
-  </si>
-  <si>
-    <t>mission_complete</t>
-  </si>
-  <si>
-    <t>Espero que te haya ido bien en tu primer dia</t>
-  </si>
-  <si>
-    <t>generic</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> @, bienvenido a Routed Inc!
+Asi conoces tu nuevo lugar de trabajo
+Por cierto, ahí arriba está la tienda de
+la ciudad, por que no compras algo
+de cable y conectores antes de 
+ir a tu trabajo?</t>
+  </si>
+  <si>
+    <t>Te envía Routed Inc? 
+Necesito que alguien haga un trabajo
+de subneteo en mi Hotel
+Te gustaríá ayudarme?</t>
+  </si>
+  <si>
+    <t>subnetting_hotel</t>
+  </si>
+  <si>
+    <t>Subnetea la red del Hotel</t>
+  </si>
+  <si>
+    <t>Has hablado con Arian, la dueña del Hotel en la ciudad de Celestia, te pidió que le ayudaras a subnetear la red de su Hotel.</t>
+  </si>
+  <si>
+    <t>Muchísimas gracias por ayudarme
+con la red de la recepción</t>
+  </si>
+  <si>
+    <t>Hola, tu eres @?
+Necesito que alguien haga un trabajo
+de subneteo en la escuela
+Te gustaríá ayudarme?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hola @, bienvenido a Routed Inc!
 Yo soy Roy
 Antes de darte un trabajo
 Prueba las estaciones de trabajo
@@ -496,65 +579,30 @@
 1 cable directo?</t>
   </si>
   <si>
-    <t>Perfecto, ahora crea:
-2 cables cruzados</t>
-  </si>
-  <si>
-    <t>cable_straight 1</t>
-  </si>
-  <si>
-    <t>cable_crossover 2</t>
-  </si>
-  <si>
-    <t>next_task</t>
-  </si>
-  <si>
-    <t>Cuentale a Roy que has creado un cable directo!</t>
-  </si>
-  <si>
-    <t>roy_crossover_cable</t>
-  </si>
-  <si>
-    <t>Cuentale a Roy que has creado dos cables cruzados!</t>
-  </si>
-  <si>
-    <t>meet_ale</t>
-  </si>
-  <si>
-    <t>Habla con Ale</t>
-  </si>
-  <si>
-    <t>Subnetea la red de la Recepcíon</t>
-  </si>
-  <si>
-    <t>roy_subnetting_reception</t>
-  </si>
-  <si>
-    <t>Vuelve con Roy</t>
-  </si>
-  <si>
-    <t>Ale te ha contado de que va este nuevo trabajo, tienes que realizar el subneteo de la Recepción, asegurate de tener los cables necesarios para comenzar.</t>
-  </si>
-  <si>
-    <t>Has terminado tu primer trabajo de subneto, vuelve a contarselo a Roy.</t>
-  </si>
-  <si>
-    <t>roy_straight_cable 1</t>
-  </si>
-  <si>
-    <t>roy_crossover_cable 1</t>
-  </si>
-  <si>
-    <t>meet_ale 1</t>
-  </si>
-  <si>
-    <t>subnetting_reception 1</t>
-  </si>
-  <si>
-    <t>roy_subnetting_reception 1</t>
-  </si>
-  <si>
-    <t>roy_straight_cable</t>
+    <t>subnetting_school</t>
+  </si>
+  <si>
+    <t>Subnetea la red de la Escuela</t>
+  </si>
+  <si>
+    <t>add_item</t>
+  </si>
+  <si>
+    <t>requirement</t>
+  </si>
+  <si>
+    <t>Como que te quedaste sin dinero?
+No te preocupes, yo te presto
+Aquí tienes!</t>
+  </si>
+  <si>
+    <t>money 200</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>poor</t>
   </si>
 </sst>
 </file>
@@ -980,17 +1028,17 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12.6" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1"/>
     <col min="5" max="5" width="34" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.44140625" style="1"/>
+    <col min="6" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1007,7 +1055,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="33.6" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -1022,12 +1070,12 @@
       </c>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -1037,7 +1085,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1052,7 +1100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
@@ -1067,7 +1115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="72" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -1082,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
@@ -1097,7 +1145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1112,7 +1160,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="50.4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" ht="54" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
@@ -1127,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="33.6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" ht="36" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -1140,7 +1188,7 @@
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1149,7 +1197,7 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1158,7 +1206,7 @@
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1167,7 +1215,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1176,7 +1224,7 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1185,14 +1233,14 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1201,7 +1249,7 @@
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1210,7 +1258,7 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1219,7 +1267,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1228,7 +1276,7 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.15">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1251,15 +1299,15 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.109375" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1321,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -1285,7 +1333,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>50</v>
       </c>
@@ -1297,7 +1345,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
@@ -1309,7 +1357,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -1321,7 +1369,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>70</v>
       </c>
@@ -1333,7 +1381,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>71</v>
       </c>
@@ -1345,7 +1393,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -1357,7 +1405,7 @@
       </c>
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
@@ -1369,7 +1417,7 @@
       </c>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
@@ -1381,7 +1429,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>59</v>
       </c>
@@ -1393,7 +1441,7 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>56</v>
       </c>
@@ -1405,7 +1453,7 @@
       </c>
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>57</v>
       </c>
@@ -1417,7 +1465,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>58</v>
       </c>
@@ -1429,7 +1477,7 @@
       </c>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>60</v>
       </c>
@@ -1441,7 +1489,7 @@
       </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>61</v>
       </c>
@@ -1453,7 +1501,7 @@
       </c>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>62</v>
       </c>
@@ -1465,7 +1513,7 @@
       </c>
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>63</v>
       </c>
@@ -1477,7 +1525,7 @@
       </c>
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>65</v>
       </c>
@@ -1489,7 +1537,7 @@
       </c>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
@@ -1501,7 +1549,7 @@
       </c>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>74</v>
       </c>
@@ -1511,19 +1559,19 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1538,22 +1586,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3A0007-EA5C-4A6A-96E9-DE9E7F963C70}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" customWidth="1"/>
-    <col min="6" max="7" width="30.6640625" customWidth="1"/>
-    <col min="8" max="8" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1567,27 +1615,27 @@
         <v>87</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>88</v>
@@ -1602,24 +1650,24 @@
         <v>80</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="84" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>52</v>
@@ -1628,24 +1676,24 @@
         <v>85</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="67.2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="72" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>65</v>
@@ -1654,13 +1702,13 @@
         <v>86</v>
       </c>
       <c r="H4" s="4" t="str">
-        <f>A5</f>
+        <f t="shared" ref="H4:H10" si="0">A5</f>
         <v>create_straight_cable</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>91</v>
@@ -1669,29 +1717,29 @@
         <v>91</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H5" s="4" t="str">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>roy_straight_cable</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>88</v>
@@ -1704,13 +1752,13 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4" t="str">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>create_crossover_cable</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>92</v>
@@ -1719,29 +1767,29 @@
         <v>92</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4" t="str">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>roy_crossover_cable</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>88</v>
@@ -1754,19 +1802,19 @@
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4" t="str">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>meet_ale</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="117.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="126" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>88</v>
@@ -1779,19 +1827,19 @@
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4" t="str">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>subnetting_reception</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="108" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>89</v>
@@ -1800,23 +1848,23 @@
         <v>63</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4" t="str">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>roy_subnetting_reception</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="54" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>88</v>
@@ -1830,15 +1878,15 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="117.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>88</v>
@@ -1848,7 +1896,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="54" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7</v>
       </c>
@@ -1865,12 +1913,10 @@
       <c r="F13" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>95</v>
-      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>8</v>
       </c>
@@ -1887,36 +1933,54 @@
       <c r="F14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>96</v>
-      </c>
+      <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="3">
-        <v>9</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>10</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>11</v>
       </c>
@@ -1928,7 +1992,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>12</v>
       </c>
@@ -1940,7 +2004,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>13</v>
       </c>
@@ -1952,7 +2016,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>14</v>
       </c>
@@ -1964,7 +2028,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>15</v>
       </c>
@@ -1976,7 +2040,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>16</v>
       </c>
@@ -1988,7 +2052,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>17</v>
       </c>
@@ -2000,7 +2064,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>18</v>
       </c>
@@ -2012,7 +2076,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>19</v>
       </c>
@@ -2024,7 +2088,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="H26" s="4"/>
     </row>
   </sheetData>
@@ -2035,22 +2099,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C18CE2-38E8-451F-BD8D-67DA76996040}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="43" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -2064,10 +2131,19 @@
         <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="139.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -2075,16 +2151,19 @@
         <v>49</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="171" customHeight="1" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="288" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -2092,16 +2171,19 @@
         <v>52</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>120</v>
+        <v>156</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="168" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:8" ht="198" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -2109,16 +2191,19 @@
         <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>139</v>
+        <v>163</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -2126,16 +2211,19 @@
         <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="67.2" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" ht="72" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -2143,16 +2231,19 @@
         <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="201.6" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="216" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -2160,16 +2251,19 @@
         <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+    </row>
+    <row r="8" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -2177,16 +2271,19 @@
         <v>63</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="134.4" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="144" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -2194,16 +2291,19 @@
         <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="E9" s="4" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -2211,16 +2311,19 @@
         <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="33.6" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2228,43 +2331,86 @@
         <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="4" t="str">
+        <f>Tasks!A15</f>
+        <v>subnetting_hotel</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="72" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="54" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -2272,8 +2418,11 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -2281,8 +2430,11 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -2290,8 +2442,11 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -2299,8 +2454,11 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-    </row>
-    <row r="19" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -2308,8 +2466,11 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-    </row>
-    <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2317,8 +2478,11 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -2326,8 +2490,11 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-    </row>
-    <row r="22" spans="1:5" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -2335,12 +2502,16 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2356,25 +2527,25 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>82</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>

<commit_message>
👷Added multiple pages for task page
</commit_message>
<xml_diff>
--- a/data/world/WiredData.xlsx
+++ b/data/world/WiredData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magic\Desktop\Wired\data\world\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF4667C2-39B4-4211-A339-1ED424D38F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6729D9-E7F0-4283-9839-F417A81FCD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{5FF7C21E-0F12-4EF8-A650-3561AF69381A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="233">
   <si>
     <t>Id</t>
   </si>
@@ -704,12 +704,6 @@
 ¿Podrías ayudarme subneteando la red del Hospital?</t>
   </si>
   <si>
-    <t>Hola, ¿tú eres name?
-Necesito que alguien haga un trabajo
-Es para subnetar la red de la escuela
-¿Te gustaría ayudarme?</t>
-  </si>
-  <si>
     <t>subnetting_hospital</t>
   </si>
   <si>
@@ -751,9 +745,6 @@
 Necesito que alguien haga un trabajo de subneteo
 ¿Es para mi Hotel, podrías ayudarme?
 Tu lugar de trabajo está en el cuarto de mi derecha</t>
-  </si>
-  <si>
-    <t>Hola, ahora necesito ayuda con el enrutamiento</t>
   </si>
   <si>
     <t>task subnetting_hotel 1</t>
@@ -835,6 +826,45 @@
   </si>
   <si>
     <t>Enrutamiento Tienda de Música</t>
+  </si>
+  <si>
+    <t>subnetting_school
+teacher</t>
+  </si>
+  <si>
+    <t>¡Hola name! 
+Gracias por haber configurado las subredes. 
+Ahora, necesitamos que configures los routers 
+Para mejorar la conectividad de los estudiantes. 
+¿Podrías encargarte de eso?</t>
+  </si>
+  <si>
+    <t>¡name! 
+Gracias por haber configurado las subredes. 
+Todavía necesitamos tu ayuda para solucionar algunos problemas 
+Especificamente de enrutamiento en nuestra red de la tienda. ¿Podrías configurar los routers?
+Es para mejorar la conectividad de los clientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ¡Gracias por tu ayuda con el subneteo 
+¿Podrías configurar los routers también? 
+Esto mejorará la conectividad de los equipos médicos</t>
+  </si>
+  <si>
+    <t>Hola, me alegra que hayas resuelto el problema de enrutamiento.
+Tenemos un problema en la red de los departamentos. 
+Los residentes no pueden acceder a Internet. 
+¿Podrías configurar los routers para solucionar el problema?</t>
+  </si>
+  <si>
+    <t>¡Hola! Soy Laura, la profesora de la escuela. 
+Si necesitas ayuda con alguna tarea o tienes alguna pregunta 
+No dudes en acercarte. Estoy aquí para apoyarte.</t>
+  </si>
+  <si>
+    <t>Si buscas instrumentos, partituras o consejos sobre música
+Estás en el lugar adecuado. 
+¡Siéntete libre de preguntarme cualquier cosa!</t>
   </si>
 </sst>
 </file>
@@ -961,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -978,9 +1008,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1538,7 +1565,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2200,7 +2227,7 @@
         <v>195</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>147</v>
@@ -2237,8 +2264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A3A0007-EA5C-4A6A-96E9-DE9E7F963C70}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -2254,25 +2281,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2527,193 +2554,193 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="16"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="16"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" ht="36" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="D15" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C16" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>219</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="16" t="s">
+      <c r="C17" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="16"/>
+    </row>
+    <row r="19" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F21" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="16"/>
-    </row>
-    <row r="16" spans="1:7" ht="36" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>219</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="G16" s="16"/>
-    </row>
-    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="G17" s="17"/>
-    </row>
-    <row r="18" spans="1:7" ht="36" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>223</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="G18" s="17"/>
-    </row>
-    <row r="19" spans="1:7" ht="36" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" s="17"/>
-    </row>
-    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" ht="36" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>222</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="17"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:7" ht="72" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -2813,11 +2840,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C18CE2-38E8-451F-BD8D-67DA76996040}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2833,178 +2860,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="1:8" ht="216" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:8" ht="252" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" ht="180" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D5" s="13" t="str">
+      <c r="D5" s="12" t="str">
         <f>Tasks!A6</f>
         <v>roy_straight_cable</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="12" t="str">
+      <c r="D6" s="11" t="str">
         <f>Tasks!G7</f>
         <v>roy_crossover_cable</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" ht="162" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="12" t="str">
+      <c r="D7" s="11" t="str">
         <f>Tasks!A9</f>
         <v>meet_ale</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" ht="36" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" ht="108" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D9" s="12" t="str">
+      <c r="D9" s="11" t="str">
         <f>Tasks!A11</f>
         <v>roy_subnetting_reception</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8" ht="36" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -3044,186 +3071,186 @@
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" ht="72" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="B12" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16" t="str">
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="str">
         <f>Tasks!A13</f>
         <v>subnetting_hotel</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="36" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16" t="s">
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="F16" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+    </row>
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="B18" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-    </row>
-    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="C15" s="16" t="s">
+      <c r="D18" s="16"/>
+      <c r="E18" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16" t="s">
-        <v>204</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-    </row>
-    <row r="16" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-    </row>
-    <row r="17" spans="1:8" ht="36" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>210</v>
-      </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-    </row>
-    <row r="18" spans="1:8" ht="72" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>211</v>
-      </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-    </row>
-    <row r="19" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17" t="s">
-        <v>224</v>
-      </c>
-      <c r="F19" s="17" t="str">
+      <c r="D19" s="16"/>
+      <c r="E19" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="16" t="str">
         <f>F15</f>
         <v>task roy_subnetting_reception 1</v>
       </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-    </row>
-    <row r="20" spans="1:8" ht="72" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="C20" s="17" t="s">
+      <c r="B20" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="C20" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -3296,84 +3323,84 @@
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10" t="str">
+      <c r="D25" s="9"/>
+      <c r="E25" s="9" t="str">
         <f>Tasks!A23</f>
         <v>chinlli</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="G25" s="11"/>
-      <c r="H25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" ht="108" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="10" t="str">
+      <c r="D26" s="9" t="str">
         <f>E25</f>
         <v>chinlli</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" ht="36" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="10" t="str">
+      <c r="D27" s="9" t="str">
         <f>Tasks!A24</f>
         <v>chinlli_2</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" ht="54" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D28" s="10" t="str">
+      <c r="D28" s="9" t="str">
         <f>Tasks!A25</f>
         <v>chinlli_3</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="H28" s="10"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" ht="54" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -3413,12 +3440,109 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+    <row r="31" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="54" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3441,129 +3565,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="8"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>4</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>5</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>4</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>